<commit_message>
all classes added, aesthetic changes to html placing
</commit_message>
<xml_diff>
--- a/Percentage Brackets and Results.xlsx
+++ b/Percentage Brackets and Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4395" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Percentage" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="74">
   <si>
     <t>ceiling</t>
   </si>
@@ -213,15 +213,6 @@
     <t>table_value</t>
   </si>
   <si>
-    <t>table1_data (object?)</t>
-  </si>
-  <si>
-    <t>table2_data (object?)</t>
-  </si>
-  <si>
-    <t>table3_data (object?)</t>
-  </si>
-  <si>
     <t>GetPercentage</t>
   </si>
   <si>
@@ -244,6 +235,21 @@
   </si>
   <si>
     <t>new getTaxRebate('table3_value', 'table3_data', 'age')</t>
+  </si>
+  <si>
+    <t>tablePercentage function</t>
+  </si>
+  <si>
+    <t>tableValue function</t>
+  </si>
+  <si>
+    <t>tableSum function</t>
+  </si>
+  <si>
+    <t>thresholdcheck</t>
+  </si>
+  <si>
+    <t>tax_value before deannualisation</t>
   </si>
 </sst>
 </file>
@@ -351,7 +357,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -456,7 +462,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -524,19 +530,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -821,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
@@ -2173,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,16 +2209,17 @@
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="79.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="103.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="103.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="30" t="s">
         <v>25</v>
@@ -2209,21 +2231,22 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="30"/>
+      <c r="I1" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
-      <c r="M1" s="31" t="s">
+      <c r="L1" s="30"/>
+      <c r="N1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="32" t="s">
+      <c r="O1" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="30"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>30</v>
       </c>
@@ -2243,17 +2266,18 @@
       <c r="G2" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="35"/>
+      <c r="I2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="31"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L2" s="31"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="31"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="31" t="s">
         <v>33</v>
@@ -2271,17 +2295,18 @@
       <c r="G3" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="35"/>
+      <c r="I3" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="31"/>
       <c r="J3" s="31"/>
       <c r="K3" s="31"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="31"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L3" s="31"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="P3" s="31"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="31"/>
       <c r="C4" s="31"/>
@@ -2289,15 +2314,16 @@
       <c r="E4" s="31"/>
       <c r="F4" s="31"/>
       <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
+      <c r="H4" s="35"/>
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="31"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L4" s="31"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="31"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="31" t="s">
         <v>36</v>
@@ -2315,45 +2341,47 @@
       <c r="G5" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="31"/>
       <c r="J5" s="31"/>
       <c r="K5" s="31"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="31"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="45" t="s">
+      <c r="L5" s="31"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="31"/>
+    </row>
+    <row r="6" spans="1:16" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="44" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="42" t="s">
+      <c r="F6" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="H6" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="M6" s="44"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="42"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H6" s="44"/>
+      <c r="I6" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
+      <c r="L6" s="45"/>
+      <c r="N6" s="46"/>
+      <c r="O6" s="46"/>
+      <c r="P6" s="44"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="31" t="s">
         <v>37</v>
@@ -2366,187 +2394,201 @@
         <v>60</v>
       </c>
       <c r="F7" s="31" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="G7" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="31"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="31" t="s">
+        <v>67</v>
+      </c>
       <c r="J7" s="31"/>
       <c r="K7" s="31"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="31"/>
-    </row>
-    <row r="8" spans="1:15" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="31"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
+      <c r="P7" s="31"/>
+    </row>
+    <row r="8" spans="1:16" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="36"/>
       <c r="B8" s="37" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="37"/>
       <c r="D8" s="37" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E8" s="38" t="s">
         <v>60</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="I8" s="37"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="37" t="s">
+        <v>68</v>
+      </c>
       <c r="J8" s="37"/>
       <c r="K8" s="37"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="40"/>
-      <c r="O8" s="37"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="31"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L8" s="37"/>
+      <c r="N8" s="42"/>
+      <c r="O8" s="42"/>
+      <c r="P8" s="37"/>
+    </row>
+    <row r="9" spans="1:16" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="48"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="32"/>
+      <c r="H9" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
+      <c r="P9" s="49"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="31" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C10" s="31"/>
       <c r="D10" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>31</v>
+        <v>54</v>
+      </c>
+      <c r="E10" s="31"/>
+      <c r="F10" s="33" t="s">
+        <v>40</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="I10" s="31"/>
+        <v>58</v>
+      </c>
+      <c r="H10" s="35"/>
+      <c r="I10" s="32" t="s">
+        <v>41</v>
+      </c>
       <c r="J10" s="31"/>
       <c r="K10" s="31"/>
-      <c r="L10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="31"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L10" s="31"/>
+      <c r="M10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="31"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="31" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="31"/>
+        <v>61</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>62</v>
+      </c>
       <c r="F11" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="35"/>
+      <c r="I11" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="I11" s="31"/>
       <c r="J11" s="31"/>
       <c r="K11" s="31"/>
-      <c r="L11" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="31"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L11" s="31"/>
+      <c r="M11" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="31"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="31" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C12" s="31"/>
       <c r="D12" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" s="31"/>
       <c r="F12" s="31" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="35"/>
+      <c r="I12" s="32" t="s">
         <v>49</v>
-      </c>
-      <c r="I12" s="34" t="s">
-        <v>51</v>
       </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>
-      <c r="L12" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="31"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L12" s="31"/>
+      <c r="M12" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="31"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
+      <c r="B13" s="31" t="s">
+        <v>51</v>
+      </c>
       <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
+      <c r="D13" s="31" t="s">
+        <v>56</v>
+      </c>
       <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
+      <c r="F13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="35"/>
+      <c r="I13" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="31"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="31"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -2554,16 +2596,17 @@
       <c r="E14" s="31"/>
       <c r="F14" s="31"/>
       <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="H14" s="35"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="31"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="31"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="31"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -2571,16 +2614,17 @@
       <c r="E15" s="31"/>
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="H15" s="35"/>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="31"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="31"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="31"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
@@ -2588,16 +2632,17 @@
       <c r="E16" s="31"/>
       <c r="F16" s="31"/>
       <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="31"/>
       <c r="J16" s="31"/>
       <c r="K16" s="31"/>
       <c r="L16" s="31"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="31"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="31"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
+      <c r="P16" s="31"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -2605,33 +2650,52 @@
       <c r="E17" s="31"/>
       <c r="F17" s="31"/>
       <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="H17" s="35"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
       <c r="K17" s="31"/>
       <c r="L17" s="31"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="31"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="M12:N12"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M3:N3"/>
-    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>